<commit_message>
Milestones and RIP updates
</commit_message>
<xml_diff>
--- a/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
+++ b/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
@@ -161,7 +161,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="4"/>
@@ -182,20 +182,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>Sheet1!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-3.2000000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-7.0999999999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -222,7 +225,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="4"/>
@@ -243,20 +246,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:f>Sheet1!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9.8000000000000004E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-5.0000000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-7.9000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -283,7 +289,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="4"/>
@@ -304,20 +310,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$6</c:f>
+              <c:f>Sheet1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8.6999999999999994E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-1E-3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-8.4000000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -344,7 +353,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="4"/>
@@ -365,20 +374,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$6</c:f>
+              <c:f>Sheet1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-1.2E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-9.6000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -396,11 +408,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44636416"/>
-        <c:axId val="50616192"/>
+        <c:axId val="98249728"/>
+        <c:axId val="98251520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="44636416"/>
+        <c:axId val="98249728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,14 +422,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50616192"/>
+        <c:crossAx val="98251520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="50616192"/>
+        <c:axId val="98251520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44636416"/>
+        <c:crossAx val="98249728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -454,16 +466,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>106878</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>249753</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -772,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,387 +838,468 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41941</v>
+        <v>42072</v>
       </c>
       <c r="B3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C3">
-        <v>9.8000000000000004E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>9.9000000000000005E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E3">
-        <v>8.7999999999999995E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>41941</v>
+        <v>42072</v>
       </c>
       <c r="I3">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="J3">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="K3">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="L3">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41912</v>
+        <v>41941</v>
       </c>
       <c r="B4">
-        <v>7.0999999999999994E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C4">
-        <v>8.2000000000000003E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D4">
-        <v>8.6999999999999994E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E4">
-        <v>0.08</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>41912</v>
+        <v>41941</v>
       </c>
       <c r="I4">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J4">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="K4">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="L4">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41878</v>
+        <v>41912</v>
       </c>
       <c r="B5">
-        <v>-3.2000000000000001E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="C5">
-        <v>-5.0000000000000001E-3</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D5">
-        <v>-1E-3</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E5">
-        <v>-1.2E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H5" s="1">
-        <v>41878</v>
+        <v>41912</v>
       </c>
       <c r="I5">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J5">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="K5">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="L5">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>41878</v>
+      </c>
+      <c r="B6">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>-1E-3</v>
+      </c>
+      <c r="E6">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>41878</v>
+      </c>
+      <c r="I6">
+        <v>213</v>
+      </c>
+      <c r="J6">
+        <v>237</v>
+      </c>
+      <c r="K6">
+        <v>250</v>
+      </c>
+      <c r="L6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>41768</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>-8.4000000000000005E-2</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <v>41768</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>196</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>218</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>230</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>7</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>8</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>41941</v>
-      </c>
-      <c r="B10">
-        <v>231</v>
-      </c>
-      <c r="C10">
-        <v>207</v>
-      </c>
-      <c r="D10">
-        <v>193</v>
-      </c>
-      <c r="E10">
-        <v>166</v>
-      </c>
-      <c r="H10" s="1">
-        <v>41941</v>
-      </c>
-      <c r="I10">
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41912</v>
+        <v>42072</v>
       </c>
       <c r="B11">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C11">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D11">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E11">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H11" s="1">
-        <v>41912</v>
+        <v>42072</v>
       </c>
       <c r="I11">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K11">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41878</v>
+        <v>41941</v>
       </c>
       <c r="B12">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C12">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="D12">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="E12">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="H12" s="1">
-        <v>41878</v>
+        <v>41941</v>
       </c>
       <c r="I12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L12">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>41912</v>
+      </c>
+      <c r="B13">
+        <v>233</v>
+      </c>
+      <c r="C13">
+        <v>208</v>
+      </c>
+      <c r="D13">
+        <v>194</v>
+      </c>
+      <c r="E13">
+        <v>167</v>
+      </c>
+      <c r="H13" s="1">
+        <v>41912</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>41878</v>
+      </c>
+      <c r="B14">
+        <v>219</v>
+      </c>
+      <c r="C14">
+        <v>195</v>
+      </c>
+      <c r="D14">
+        <v>182</v>
+      </c>
+      <c r="E14">
+        <v>155</v>
+      </c>
+      <c r="H14" s="1">
+        <v>41878</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>41768</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>197</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>175</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>163</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>138</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H15" s="1">
         <v>41768</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>2</v>
       </c>
-      <c r="J13">
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="L15">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>41941</v>
-      </c>
-      <c r="B17">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>23</v>
-      </c>
-      <c r="E17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>41912</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>19</v>
-      </c>
-      <c r="E18">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41878</v>
+        <v>42072</v>
       </c>
       <c r="B19">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>41912</v>
+      </c>
+      <c r="B21">
         <v>16</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
+        <v>41878</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>41768</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>0</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed model genes misalignment
</commit_message>
<xml_diff>
--- a/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
+++ b/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15576" windowHeight="9816"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15570" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,16 @@
     <t>Case 1</t>
   </si>
   <si>
-    <t>MCC = TP*TN-FP*FN/sqrt((TP+FP)(TP+FN)(TN+FP)(TN+FN)</t>
+    <t>ACC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,9 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,20 +169,26 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="d\-mmm">
+                  <c:v>42269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42072</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>41941</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>41912</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>41878</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>41768</c:v>
                 </c:pt>
               </c:numCache>
@@ -185,23 +196,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.29099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-3.2000000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-7.0999999999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -228,20 +242,26 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="d\-mmm">
+                  <c:v>42269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42072</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>41941</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>41912</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>41878</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>41768</c:v>
                 </c:pt>
               </c:numCache>
@@ -249,23 +269,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$7</c:f>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9.8000000000000004E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-5.0000000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-7.9000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -292,20 +315,26 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="d\-mmm">
+                  <c:v>42269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42072</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>41941</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>41912</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>41878</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>41768</c:v>
                 </c:pt>
               </c:numCache>
@@ -313,23 +342,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$7</c:f>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5.2999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8.6999999999999994E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-1E-3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-8.4000000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -356,20 +388,26 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="d\-mmm">
+                  <c:v>42269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42072</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>41941</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>41912</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>41878</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>41768</c:v>
                 </c:pt>
               </c:numCache>
@@ -377,23 +415,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$7</c:f>
+              <c:f>Sheet1!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.28899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-1.2E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-9.6000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -411,28 +452,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134850816"/>
-        <c:axId val="134860800"/>
+        <c:axId val="75207424"/>
+        <c:axId val="75208960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="134850816"/>
+        <c:axId val="75207424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134860800"/>
+        <c:crossAx val="75208960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="134860800"/>
+        <c:axId val="75208960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134850816"/>
+        <c:crossAx val="75207424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -469,16 +510,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>249753</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>78303</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -787,19 +828,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -807,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -839,513 +880,689 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42269</v>
+      </c>
+      <c r="B3">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E3">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="H3" s="2">
+        <v>42269</v>
+      </c>
+      <c r="I3">
+        <v>110</v>
+      </c>
+      <c r="J3">
+        <v>123</v>
+      </c>
+      <c r="K3">
+        <v>134</v>
+      </c>
+      <c r="L3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>42072</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0.02</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H4" s="1">
         <v>42072</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>220</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>244</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>257</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>41941</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="1">
         <v>41941</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>213</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <v>237</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>251</v>
       </c>
-      <c r="L4">
+      <c r="L5">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>41912</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>0.08</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H6" s="1">
         <v>41912</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>216</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <v>241</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <v>255</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>41878</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>-3.2000000000000001E-2</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>-1E-3</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>-1.2E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H7" s="1">
         <v>41878</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>213</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>237</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>250</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>41768</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>-8.4000000000000005E-2</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H8" s="1">
         <v>41768</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>196</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <v>218</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>230</v>
       </c>
-      <c r="L7">
+      <c r="L8">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>7</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>8</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>42269</v>
+      </c>
+      <c r="B12">
+        <v>204</v>
+      </c>
+      <c r="C12">
+        <v>191</v>
+      </c>
+      <c r="D12">
+        <v>180</v>
+      </c>
+      <c r="E12">
+        <v>155</v>
+      </c>
+      <c r="H12" s="2">
+        <v>42269</v>
+      </c>
+      <c r="I12">
+        <v>81</v>
+      </c>
+      <c r="J12">
+        <v>63</v>
+      </c>
+      <c r="K12">
+        <v>55</v>
+      </c>
+      <c r="L12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>42072</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>228</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>204</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>191</v>
       </c>
-      <c r="E11">
+      <c r="E13">
         <v>164</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H13" s="1">
         <v>42072</v>
       </c>
-      <c r="I11">
+      <c r="I13">
         <v>16</v>
       </c>
-      <c r="J11">
+      <c r="J13">
         <v>13</v>
       </c>
-      <c r="K11">
+      <c r="K13">
         <v>11</v>
       </c>
-      <c r="L11">
+      <c r="L13">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>41941</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>231</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>207</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>193</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>166</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H14" s="1">
         <v>41941</v>
       </c>
-      <c r="I12">
+      <c r="I14">
         <v>11</v>
       </c>
-      <c r="J12">
+      <c r="J14">
         <v>8</v>
       </c>
-      <c r="K12">
+      <c r="K14">
         <v>7</v>
       </c>
-      <c r="L12">
+      <c r="L14">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>41912</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>233</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>208</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>194</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>167</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H15" s="1">
         <v>41912</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="J15">
         <v>7</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>6</v>
       </c>
-      <c r="L13">
+      <c r="L15">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>41878</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>219</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>195</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>182</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>155</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H16" s="1">
         <v>41878</v>
       </c>
-      <c r="I14">
+      <c r="I16">
         <v>15</v>
       </c>
-      <c r="J14">
+      <c r="J16">
         <v>12</v>
       </c>
-      <c r="K14">
+      <c r="K16">
         <v>11</v>
       </c>
-      <c r="L14">
+      <c r="L16">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>41768</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>197</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>175</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>163</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>138</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H17" s="1">
         <v>41768</v>
       </c>
-      <c r="I15">
+      <c r="I17">
         <v>2</v>
       </c>
-      <c r="J15">
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="K15">
+      <c r="K17">
         <v>2</v>
       </c>
-      <c r="L15">
+      <c r="L17">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>42269</v>
+      </c>
+      <c r="B21">
+        <v>147</v>
+      </c>
+      <c r="C21">
+        <v>165</v>
+      </c>
+      <c r="D21">
+        <v>173</v>
+      </c>
+      <c r="E21">
+        <v>180</v>
+      </c>
+      <c r="H21" s="2">
+        <v>42269</v>
+      </c>
+      <c r="I21" s="3">
+        <f>100*(B12+B21)/(B12+B21+I12+I3)</f>
+        <v>64.760147601476021</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" ref="J21" si="0">100*(C12+C21)/(C12+C21+J12+J3)</f>
+        <v>65.682656826568262</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" ref="K21" si="1">100*(D12+D21)/(D12+D21+K12+K3)</f>
+        <v>65.129151291512912</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" ref="L21" si="2">100*(E12+E21)/(E12+E21+L12+L3)</f>
+        <v>61.808118081180815</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>42072</v>
       </c>
-      <c r="B19">
+      <c r="B22">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <v>21</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <v>23</v>
       </c>
-      <c r="E19">
+      <c r="E22">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="H22" s="1">
+        <v>42072</v>
+      </c>
+      <c r="I22" s="3">
+        <f>100*(B13+B22)/(B13+B22+I13+I4)</f>
+        <v>51.037344398340252</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" ref="J22:L23" si="3">100*(C13+C22)/(C13+C22+J13+J4)</f>
+        <v>46.680497925311201</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="3"/>
+        <v>44.398340248962654</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="3"/>
+        <v>39.004149377593365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>41941</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>22</v>
       </c>
-      <c r="D20">
+      <c r="D23">
         <v>23</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+      <c r="H23" s="1">
+        <v>41941</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" ref="I23:I26" si="4">100*(B14+B23)/(B14+B23+I14+I5)</f>
+        <v>52.742616033755276</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="3"/>
+        <v>48.312236286919834</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="3"/>
+        <v>45.569620253164558</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="3"/>
+        <v>40.084388185654007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>41912</v>
       </c>
-      <c r="B21">
+      <c r="B24">
         <v>16</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>18</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>19</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>20</v>
       </c>
-      <c r="I21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+      <c r="H24" s="1">
+        <v>41912</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="4"/>
+        <v>52.531645569620252</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" ref="J24:J26" si="5">100*(C15+C24)/(C15+C24+J15+J6)</f>
+        <v>47.679324894514771</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ref="K24:K26" si="6">100*(D15+D24)/(D15+D24+K15+K6)</f>
+        <v>44.936708860759495</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" ref="L24:L26" si="7">100*(E15+E24)/(E15+E24+L15+L6)</f>
+        <v>39.451476793248943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>41878</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <v>11</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>14</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>15</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>16</v>
       </c>
-      <c r="I22">
-        <v>25</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-      <c r="L22">
+      <c r="H25" s="1">
+        <v>41878</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="4"/>
+        <v>50.21834061135371</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="5"/>
+        <v>45.633187772925766</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="6"/>
+        <v>43.013100436681221</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="7"/>
+        <v>37.336244541484717</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>41768</v>
+      </c>
+      <c r="B26">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
         <v>41768</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H28">
-        <f>(I22*J22-K22*L22)/SQRT((I22+K22)*(I22+L22)*(J22+K22)*(J22+L22))</f>
-        <v>0.59761430466719678</v>
-      </c>
-    </row>
+      <c r="I26" s="3">
+        <f t="shared" si="4"/>
+        <v>49.87341772151899</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="5"/>
+        <v>44.303797468354432</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="6"/>
+        <v>41.265822784810126</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="7"/>
+        <v>34.936708860759495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1359,7 +1576,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1371,7 +1588,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lots of code cleanup
</commit_message>
<xml_diff>
--- a/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
+++ b/Matt_Work/Gene Essentiality/MCC Evolution.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$53</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>MCC</t>
   </si>
@@ -56,7 +59,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -91,7 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,11 +455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="75207424"/>
-        <c:axId val="75208960"/>
+        <c:axId val="99723520"/>
+        <c:axId val="99729408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75207424"/>
+        <c:axId val="99723520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,14 +469,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75208960"/>
+        <c:crossAx val="99729408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75208960"/>
+        <c:axId val="99729408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75207424"/>
+        <c:crossAx val="99723520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -510,16 +513,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>78303</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -828,27 +831,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -864,23 +867,20 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42269</v>
       </c>
@@ -896,23 +896,20 @@
       <c r="E3">
         <v>0.28899999999999998</v>
       </c>
-      <c r="H3" s="2">
-        <v>42269</v>
+      <c r="G3">
+        <v>110</v>
+      </c>
+      <c r="H3">
+        <v>123</v>
       </c>
       <c r="I3">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="J3">
-        <v>123</v>
-      </c>
-      <c r="K3">
-        <v>134</v>
-      </c>
-      <c r="L3">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42072</v>
       </c>
@@ -928,23 +925,20 @@
       <c r="E4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H4" s="1">
-        <v>42072</v>
+      <c r="G4">
+        <v>220</v>
+      </c>
+      <c r="H4">
+        <v>244</v>
       </c>
       <c r="I4">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="J4">
-        <v>244</v>
-      </c>
-      <c r="K4">
-        <v>257</v>
-      </c>
-      <c r="L4">
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>41941</v>
       </c>
@@ -960,23 +954,20 @@
       <c r="E5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="H5" s="1">
-        <v>41941</v>
+      <c r="G5">
+        <v>213</v>
+      </c>
+      <c r="H5">
+        <v>237</v>
       </c>
       <c r="I5">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="J5">
-        <v>237</v>
-      </c>
-      <c r="K5">
-        <v>251</v>
-      </c>
-      <c r="L5">
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41912</v>
       </c>
@@ -992,23 +983,20 @@
       <c r="E6">
         <v>0.08</v>
       </c>
-      <c r="H6" s="1">
-        <v>41912</v>
+      <c r="G6">
+        <v>216</v>
+      </c>
+      <c r="H6">
+        <v>241</v>
       </c>
       <c r="I6">
-        <v>216</v>
+        <v>255</v>
       </c>
       <c r="J6">
-        <v>241</v>
-      </c>
-      <c r="K6">
-        <v>255</v>
-      </c>
-      <c r="L6">
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41878</v>
       </c>
@@ -1024,23 +1012,20 @@
       <c r="E7">
         <v>-1.2E-2</v>
       </c>
-      <c r="H7" s="1">
-        <v>41878</v>
+      <c r="G7">
+        <v>213</v>
+      </c>
+      <c r="H7">
+        <v>237</v>
       </c>
       <c r="I7">
-        <v>213</v>
+        <v>250</v>
       </c>
       <c r="J7">
-        <v>237</v>
-      </c>
-      <c r="K7">
-        <v>250</v>
-      </c>
-      <c r="L7">
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41768</v>
       </c>
@@ -1056,31 +1041,28 @@
       <c r="E8">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="H8" s="1">
-        <v>41768</v>
+      <c r="G8">
+        <v>196</v>
+      </c>
+      <c r="H8">
+        <v>218</v>
       </c>
       <c r="I8">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="J8">
-        <v>218</v>
-      </c>
-      <c r="K8">
-        <v>230</v>
-      </c>
-      <c r="L8">
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1096,23 +1078,20 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
       <c r="H11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42269</v>
       </c>
@@ -1128,23 +1107,20 @@
       <c r="E12">
         <v>155</v>
       </c>
-      <c r="H12" s="2">
-        <v>42269</v>
+      <c r="G12">
+        <v>81</v>
+      </c>
+      <c r="H12">
+        <v>63</v>
       </c>
       <c r="I12">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="J12">
-        <v>63</v>
-      </c>
-      <c r="K12">
-        <v>55</v>
-      </c>
-      <c r="L12">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42072</v>
       </c>
@@ -1160,23 +1136,20 @@
       <c r="E13">
         <v>164</v>
       </c>
-      <c r="H13" s="1">
-        <v>42072</v>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
       </c>
       <c r="I13">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J13">
-        <v>13</v>
-      </c>
-      <c r="K13">
-        <v>11</v>
-      </c>
-      <c r="L13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>41941</v>
       </c>
@@ -1192,23 +1165,20 @@
       <c r="E14">
         <v>166</v>
       </c>
-      <c r="H14" s="1">
-        <v>41941</v>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
       </c>
       <c r="I14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J14">
-        <v>8</v>
-      </c>
-      <c r="K14">
-        <v>7</v>
-      </c>
-      <c r="L14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>41912</v>
       </c>
@@ -1224,23 +1194,20 @@
       <c r="E15">
         <v>167</v>
       </c>
-      <c r="H15" s="1">
-        <v>41912</v>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J15">
-        <v>7</v>
-      </c>
-      <c r="K15">
-        <v>6</v>
-      </c>
-      <c r="L15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>41878</v>
       </c>
@@ -1256,23 +1223,20 @@
       <c r="E16">
         <v>155</v>
       </c>
-      <c r="H16" s="1">
-        <v>41878</v>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
       </c>
       <c r="I16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J16">
-        <v>12</v>
-      </c>
-      <c r="K16">
-        <v>11</v>
-      </c>
-      <c r="L16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>41768</v>
       </c>
@@ -1288,8 +1252,11 @@
       <c r="E17">
         <v>138</v>
       </c>
-      <c r="H17" s="1">
-        <v>41768</v>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1297,22 +1264,16 @@
       <c r="J17">
         <v>2</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1328,23 +1289,20 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
       <c r="H20" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42269</v>
       </c>
@@ -1360,27 +1318,24 @@
       <c r="E21">
         <v>180</v>
       </c>
-      <c r="H21" s="2">
-        <v>42269</v>
+      <c r="G21" s="3">
+        <f>100*(B12+B21)/(B12+B21+G12+G3)</f>
+        <v>64.760147601476021</v>
+      </c>
+      <c r="H21" s="3">
+        <f>100*(C12+C21)/(C12+C21+H12+H3)</f>
+        <v>65.682656826568262</v>
       </c>
       <c r="I21" s="3">
-        <f>100*(B12+B21)/(B12+B21+I12+I3)</f>
-        <v>64.760147601476021</v>
+        <f>100*(D12+D21)/(D12+D21+I12+I3)</f>
+        <v>65.129151291512912</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" ref="J21" si="0">100*(C12+C21)/(C12+C21+J12+J3)</f>
-        <v>65.682656826568262</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" ref="K21" si="1">100*(D12+D21)/(D12+D21+K12+K3)</f>
-        <v>65.129151291512912</v>
-      </c>
-      <c r="L21" s="3">
-        <f t="shared" ref="L21" si="2">100*(E12+E21)/(E12+E21+L12+L3)</f>
+        <f>100*(E12+E21)/(E12+E21+J12+J3)</f>
         <v>61.808118081180815</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42072</v>
       </c>
@@ -1396,27 +1351,24 @@
       <c r="E22">
         <v>24</v>
       </c>
-      <c r="H22" s="1">
-        <v>42072</v>
+      <c r="G22" s="3">
+        <f>100*(B13+B22)/(B13+B22+G13+G4)</f>
+        <v>51.037344398340252</v>
+      </c>
+      <c r="H22" s="3">
+        <f>100*(C13+C22)/(C13+C22+H13+H4)</f>
+        <v>46.680497925311201</v>
       </c>
       <c r="I22" s="3">
-        <f>100*(B13+B22)/(B13+B22+I13+I4)</f>
-        <v>51.037344398340252</v>
+        <f>100*(D13+D22)/(D13+D22+I13+I4)</f>
+        <v>44.398340248962654</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ref="J22:L23" si="3">100*(C13+C22)/(C13+C22+J13+J4)</f>
-        <v>46.680497925311201</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="3"/>
-        <v>44.398340248962654</v>
-      </c>
-      <c r="L22" s="3">
-        <f t="shared" si="3"/>
+        <f>100*(E13+E22)/(E13+E22+J13+J4)</f>
         <v>39.004149377593365</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>41941</v>
       </c>
@@ -1432,27 +1384,24 @@
       <c r="E23">
         <v>24</v>
       </c>
-      <c r="H23" s="1">
-        <v>41941</v>
+      <c r="G23" s="3">
+        <f>100*(B14+B23)/(B14+B23+G14+G5)</f>
+        <v>52.742616033755276</v>
+      </c>
+      <c r="H23" s="3">
+        <f>100*(C14+C23)/(C14+C23+H14+H5)</f>
+        <v>48.312236286919834</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" ref="I23:I26" si="4">100*(B14+B23)/(B14+B23+I14+I5)</f>
-        <v>52.742616033755276</v>
+        <f>100*(D14+D23)/(D14+D23+I14+I5)</f>
+        <v>45.569620253164558</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="3"/>
-        <v>48.312236286919834</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="3"/>
-        <v>45.569620253164558</v>
-      </c>
-      <c r="L23" s="3">
-        <f t="shared" si="3"/>
+        <f>100*(E14+E23)/(E14+E23+J14+J5)</f>
         <v>40.084388185654007</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>41912</v>
       </c>
@@ -1468,27 +1417,24 @@
       <c r="E24">
         <v>20</v>
       </c>
-      <c r="H24" s="1">
-        <v>41912</v>
+      <c r="G24" s="3">
+        <f>100*(B15+B24)/(B15+B24+G15+G6)</f>
+        <v>52.531645569620252</v>
+      </c>
+      <c r="H24" s="3">
+        <f>100*(C15+C24)/(C15+C24+H15+H6)</f>
+        <v>47.679324894514771</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="4"/>
-        <v>52.531645569620252</v>
+        <f>100*(D15+D24)/(D15+D24+I15+I6)</f>
+        <v>44.936708860759495</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" ref="J24:J26" si="5">100*(C15+C24)/(C15+C24+J15+J6)</f>
-        <v>47.679324894514771</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" ref="K24:K26" si="6">100*(D15+D24)/(D15+D24+K15+K6)</f>
-        <v>44.936708860759495</v>
-      </c>
-      <c r="L24" s="3">
-        <f t="shared" ref="L24:L26" si="7">100*(E15+E24)/(E15+E24+L15+L6)</f>
+        <f>100*(E15+E24)/(E15+E24+J15+J6)</f>
         <v>39.451476793248943</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>41878</v>
       </c>
@@ -1504,27 +1450,24 @@
       <c r="E25">
         <v>16</v>
       </c>
-      <c r="H25" s="1">
-        <v>41878</v>
+      <c r="G25" s="3">
+        <f>100*(B16+B25)/(B16+B25+G16+G7)</f>
+        <v>50.21834061135371</v>
+      </c>
+      <c r="H25" s="3">
+        <f>100*(C16+C25)/(C16+C25+H16+H7)</f>
+        <v>45.633187772925766</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="4"/>
-        <v>50.21834061135371</v>
+        <f>100*(D16+D25)/(D16+D25+I16+I7)</f>
+        <v>43.013100436681221</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="5"/>
-        <v>45.633187772925766</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="6"/>
-        <v>43.013100436681221</v>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" si="7"/>
+        <f>100*(E16+E25)/(E16+E25+J16+J7)</f>
         <v>37.336244541484717</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>41768</v>
       </c>
@@ -1540,32 +1483,26 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="H26" s="1">
-        <v>41768</v>
+      <c r="G26" s="3">
+        <f>100*(B17+B26)/(B17+B26+G17+G8)</f>
+        <v>49.87341772151899</v>
+      </c>
+      <c r="H26" s="3">
+        <f>100*(C17+C26)/(C17+C26+H17+H8)</f>
+        <v>44.303797468354432</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="4"/>
-        <v>49.87341772151899</v>
+        <f>100*(D17+D26)/(D17+D26+I17+I8)</f>
+        <v>41.265822784810126</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="5"/>
-        <v>44.303797468354432</v>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" si="6"/>
-        <v>41.265822784810126</v>
-      </c>
-      <c r="L26" s="3">
-        <f t="shared" si="7"/>
+        <f>100*(E17+E26)/(E17+E26+J17+J8)</f>
         <v>34.936708860759495</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:12" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>